<commit_message>
KMAA Permisos y auditoria
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\RRHH\djangular_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects Repository\djangular_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2E9CD2-DBB0-4833-B1AE-7C8C50EE3B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EB612F-1BF5-42A2-BA8A-B65EF495008B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CA9618F9-43CD-4C24-B4D7-1F73EAFD6C89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA9618F9-43CD-4C24-B4D7-1F73EAFD6C89}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="120">
   <si>
     <t>id</t>
   </si>
@@ -147,15 +147,6 @@
     <t>increments</t>
   </si>
   <si>
-    <t>auth_user</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Máximo de reservas por semana</t>
-  </si>
-  <si>
     <t>weekly_max_bookings</t>
   </si>
   <si>
@@ -232,9 +223,6 @@
   </si>
   <si>
     <t>Hora inicial del intervalo disponible en el día determinado por el eschedule_id</t>
-  </si>
-  <si>
-    <t>Esto se puede establecer en la config del espacio</t>
   </si>
   <si>
     <t>Máximo de reservas en la semana por usuario</t>
@@ -512,10 +500,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,26 +818,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D53CC1-B88A-432E-84F9-3425553A8C93}">
-  <dimension ref="B3:E57"/>
+  <dimension ref="B3:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A44" sqref="A44:XFD48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="86.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="86.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -860,10 +848,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -874,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -885,7 +873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -896,10 +884,10 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -907,10 +895,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>29</v>
       </c>
@@ -921,7 +909,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
@@ -929,74 +917,74 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -1018,7 +1006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1029,12 +1017,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1045,10 +1033,10 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -1059,12 +1047,12 @@
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -1073,10 +1061,10 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>17</v>
       </c>
@@ -1087,7 +1075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -1098,10 +1086,10 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -1112,10 +1100,10 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>9</v>
       </c>
@@ -1126,7 +1114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>10</v>
       </c>
@@ -1137,7 +1125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>11</v>
       </c>
@@ -1148,15 +1136,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>21</v>
       </c>
@@ -1167,10 +1155,10 @@
         <v>2</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
@@ -1181,7 +1169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1180,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
@@ -1203,21 +1191,21 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
         <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>9</v>
       </c>
@@ -1228,7 +1216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>10</v>
       </c>
@@ -1239,7 +1227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>11</v>
       </c>
@@ -1250,128 +1238,90 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
-        <v>39</v>
+      <c r="E46" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>0</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
         <v>38</v>
       </c>
-      <c r="E47" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="C48" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>41</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D48" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="D49" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>18</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C50" t="s">
         <v>20</v>
       </c>
-      <c r="D55" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="7" t="s">
+      <c r="D50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C51" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D51" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="7" t="s">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C52" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>71</v>
+      <c r="D52" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1388,17 +1338,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1409,10 +1359,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -1423,7 +1373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -1431,10 +1381,10 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -1445,7 +1395,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -1456,7 +1406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -1467,12 +1417,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1483,10 +1433,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -1497,9 +1447,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1508,15 +1458,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1528,357 +1478,357 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623545E4-263D-4384-8CE9-8E7CA32C371D}">
   <dimension ref="B4:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="1.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="1.88671875" style="11" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4.5546875" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" customWidth="1"/>
+    <col min="11" max="11" width="4.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="14"/>
+        <v>73</v>
+      </c>
+      <c r="G4" s="13"/>
       <c r="I4" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G6" s="11"/>
       <c r="I6" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
         <v>80</v>
       </c>
-      <c r="I7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I20" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>121</v>
-      </c>
-      <c r="I9" t="s">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="J21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C22" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="29" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J10" t="s">
+      <c r="I29" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+      <c r="J30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="J34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>119</v>
+      </c>
+      <c r="J35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I39" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J11" t="s">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J41" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I45" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J47" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="9:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="I51" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="J52" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="J21" t="s">
+    <row r="53" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="K53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="K59" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-    </row>
-    <row r="29" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>91</v>
-      </c>
-      <c r="J30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>90</v>
-      </c>
-      <c r="J34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>123</v>
-      </c>
-      <c r="J35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I39" s="12" t="s">
+    <row r="60" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L60" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L61" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="L63" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="J64" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J42" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I45" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J47" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J48" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="9:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I51" s="12" t="s">
+    <row r="65" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K65" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L66" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="J52" s="1" t="s">
+    <row r="67" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L67" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L68" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L69" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L70" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L71" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K72" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="73" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L73" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="10:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L74" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="J75" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="K76" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="K53" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L54" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L55" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L57" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L58" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="K59" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="60" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L61" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="62" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L62" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="L63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="J64" s="1" t="s">
+    <row r="77" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L77" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="K65" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L66" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="67" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L67" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="68" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L68" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="69" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L69" t="s">
+    <row r="78" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L78" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L70" t="s">
+    <row r="79" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L79" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="71" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L71" t="s">
+    <row r="80" spans="10:12" x14ac:dyDescent="0.3">
+      <c r="L80" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="72" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="K72" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L73" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="74" spans="10:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L74" t="s">
+    <row r="81" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K81" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L82" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="83" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L83" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="75" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J75" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="76" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="K76" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="77" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L77" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="78" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L78" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="79" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L79" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="80" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L80" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="81" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K81" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="L82" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="83" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="L83" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KMAA reusable data table
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects Repository\djangular_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\RRHH\djangular_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EB612F-1BF5-42A2-BA8A-B65EF495008B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EA2D9F-54C8-41F2-9AF3-5B6246B154B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA9618F9-43CD-4C24-B4D7-1F73EAFD6C89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{CA9618F9-43CD-4C24-B4D7-1F73EAFD6C89}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="121">
   <si>
     <t>id</t>
   </si>
@@ -324,15 +324,9 @@
     <t>Detalle de reservas</t>
   </si>
   <si>
-    <t>Usuarios</t>
-  </si>
-  <si>
     <t>REPORTES (EXCEL)</t>
   </si>
   <si>
-    <t>Resumen de reservas</t>
-  </si>
-  <si>
     <t>Columnas</t>
   </si>
   <si>
@@ -397,13 +391,22 @@
   </si>
   <si>
     <t>Editar (correo, contraseña, nombres)</t>
+  </si>
+  <si>
+    <t>Usuarios (NO)</t>
+  </si>
+  <si>
+    <t>Resumen de reservas (NO)</t>
+  </si>
+  <si>
+    <t>IMAGEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,6 +450,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -486,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -504,6 +515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,24 +832,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D53CC1-B88A-432E-84F9-3425553A8C93}">
   <dimension ref="B3:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A44" sqref="A44:XFD48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="86.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="86.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -851,7 +863,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -862,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -873,7 +885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -887,7 +899,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -898,7 +910,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>29</v>
       </c>
@@ -909,7 +921,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
@@ -920,7 +932,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>44</v>
       </c>
@@ -931,7 +943,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>37</v>
       </c>
@@ -945,7 +957,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
@@ -959,7 +971,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>64</v>
       </c>
@@ -973,7 +985,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>51</v>
       </c>
@@ -984,7 +996,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>9</v>
       </c>
@@ -995,7 +1007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1018,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -1017,12 +1029,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1036,7 +1048,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1062,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>43</v>
       </c>
@@ -1064,7 +1076,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +1087,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>18</v>
       </c>
@@ -1089,7 +1101,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>19</v>
       </c>
@@ -1103,7 +1115,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>9</v>
       </c>
@@ -1114,7 +1126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>10</v>
       </c>
@@ -1125,7 +1137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>11</v>
       </c>
@@ -1136,7 +1148,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
@@ -1144,7 +1156,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>21</v>
       </c>
@@ -1158,7 +1170,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
@@ -1169,7 +1181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1192,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
@@ -1191,7 +1203,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>65</v>
       </c>
@@ -1205,7 +1217,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>9</v>
       </c>
@@ -1216,7 +1228,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>10</v>
       </c>
@@ -1227,7 +1239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>11</v>
       </c>
@@ -1238,12 +1250,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>21</v>
       </c>
@@ -1257,7 +1269,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1281,7 @@
       </c>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>38</v>
       </c>
@@ -1280,7 +1292,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
         <v>47</v>
       </c>
@@ -1291,7 +1303,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>18</v>
       </c>
@@ -1302,7 +1314,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
         <v>19</v>
       </c>
@@ -1313,7 +1325,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="s">
         <v>28</v>
       </c>
@@ -1338,17 +1350,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -1384,7 +1396,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -1395,7 +1407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -1406,7 +1418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -1417,12 +1429,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -1447,7 +1459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>43</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>56</v>
       </c>
@@ -1478,23 +1490,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623545E4-263D-4384-8CE9-8E7CA32C371D}">
   <dimension ref="B4:L83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="1.88671875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" style="11" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="4.5546875" customWidth="1"/>
-    <col min="10" max="10" width="5.88671875" customWidth="1"/>
-    <col min="11" max="11" width="4.88671875" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>73</v>
       </c>
@@ -1503,7 +1515,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>75</v>
       </c>
@@ -1512,7 +1524,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>76</v>
       </c>
@@ -1520,7 +1532,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>77</v>
       </c>
@@ -1528,35 +1540,35 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>81</v>
       </c>
@@ -1564,7 +1576,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>88</v>
       </c>
@@ -1572,21 +1584,21 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C22" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
     </row>
-    <row r="29" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
         <v>82</v>
       </c>
@@ -1594,7 +1606,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>87</v>
       </c>
@@ -1602,15 +1614,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>86</v>
       </c>
@@ -1618,217 +1630,223 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J35" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I39" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J41" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I45" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J47" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="9:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I51" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="9:12" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="9:12" x14ac:dyDescent="0.25">
       <c r="J52" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K53" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L55" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="L54" t="s">
+    <row r="56" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L56" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="L55" t="s">
+    <row r="57" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L57" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="L56" t="s">
+    <row r="58" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L58" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="L57" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="58" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="L58" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="9:12" x14ac:dyDescent="0.25">
       <c r="K59" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="9:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="9:12" x14ac:dyDescent="0.25">
       <c r="L60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L61" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="L63" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="L61" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="62" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="L62" t="s">
+    <row r="64" spans="9:12" x14ac:dyDescent="0.25">
+      <c r="J64" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K65" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L66" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L67" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="63" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="L63" t="s">
+    <row r="68" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L68" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="9:12" x14ac:dyDescent="0.3">
-      <c r="J64" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="65" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="K65" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="66" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L66" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L67" t="s">
+    <row r="69" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L69" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L68" t="s">
+    <row r="70" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L70" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L69" t="s">
+    <row r="71" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L71" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L70" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="71" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L71" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="72" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K72" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="73" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="10:12" x14ac:dyDescent="0.25">
       <c r="L73" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="10:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L74" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J75" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="76" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J76" s="6"/>
+      <c r="K76" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L77" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L78" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L79" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="10:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L74" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="75" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="J75" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="76" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="K76" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L78" t="s">
+    <row r="80" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L80" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L79" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="80" spans="10:12" x14ac:dyDescent="0.3">
-      <c r="L80" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K81" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="11:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="11:12" x14ac:dyDescent="0.25">
       <c r="L82" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="83" spans="11:12" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="83" spans="11:12" x14ac:dyDescent="0.25">
       <c r="L83" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>